<commit_message>
edit graphs for report
</commit_message>
<xml_diff>
--- a/Results/Graphs_report2/tables.xlsx
+++ b/Results/Graphs_report2/tables.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>year</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>ERC_PR</t>
+  </si>
+  <si>
+    <t>NC_PR</t>
   </si>
   <si>
     <t>ExF_MA</t>
@@ -227,10 +230,13 @@
       <c r="M1" t="s">
         <v>11</v>
       </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" t="n">
         <v>2015.0</v>
@@ -263,15 +269,18 @@
         <v>31.43888383974378</v>
       </c>
       <c r="L2" t="n">
+        <v>28.233351474359893</v>
+      </c>
+      <c r="M2" t="n">
         <v>-1.6694337658040215</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>12.26596018288873</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="n">
         <v>2016.0</v>
@@ -304,15 +313,18 @@
         <v>29.609159141489314</v>
       </c>
       <c r="L3" t="n">
+        <v>26.834264792199534</v>
+      </c>
+      <c r="M3" t="n">
         <v>-1.777756714551622</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>11.97799542009921</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="n">
         <v>2017.0</v>
@@ -345,15 +357,18 @@
         <v>26.72053262749625</v>
       </c>
       <c r="L4" t="n">
+        <v>25.93219265135643</v>
+      </c>
+      <c r="M4" t="n">
         <v>-2.017035801511651</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>11.86474487237708</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" t="n">
         <v>2018.0</v>
@@ -386,15 +401,18 @@
         <v>26.22867130436302</v>
       </c>
       <c r="L5" t="n">
+        <v>25.077051653222373</v>
+      </c>
+      <c r="M5" t="n">
         <v>-2.0519218502833345</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>11.722075209578518</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="n">
         <v>2019.0</v>
@@ -427,15 +445,18 @@
         <v>23.986241294949124</v>
       </c>
       <c r="L6" t="n">
+        <v>24.25923049405211</v>
+      </c>
+      <c r="M6" t="n">
         <v>-2.2342408360497346</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
         <v>11.577002011274585</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" t="n">
         <v>2020.0</v>
@@ -468,15 +489,18 @@
         <v>21.15083417394243</v>
       </c>
       <c r="L7" t="n">
+        <v>23.785146651455086</v>
+      </c>
+      <c r="M7" t="n">
         <v>-2.2477383265021826</v>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
         <v>11.567780073910502</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" t="n">
         <v>2021.0</v>
@@ -509,15 +533,18 @@
         <v>20.7519140838895</v>
       </c>
       <c r="L8" t="n">
+        <v>23.68823758525744</v>
+      </c>
+      <c r="M8" t="n">
         <v>-2.3765392287708633</v>
       </c>
-      <c r="M8" t="n">
+      <c r="N8" t="n">
         <v>11.745260871036011</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" t="n">
         <v>2022.0</v>
@@ -550,15 +577,18 @@
         <v>20.670662643955207</v>
       </c>
       <c r="L9" t="n">
+        <v>23.60056645324508</v>
+      </c>
+      <c r="M9" t="n">
         <v>-2.4654454245635287</v>
       </c>
-      <c r="M9" t="n">
+      <c r="N9" t="n">
         <v>11.903903298795349</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" t="n">
         <v>2023.0</v>
@@ -591,15 +621,18 @@
         <v>20.608337378625027</v>
       </c>
       <c r="L10" t="n">
+        <v>23.51953724194511</v>
+      </c>
+      <c r="M10" t="n">
         <v>-2.544783501628456</v>
       </c>
-      <c r="M10" t="n">
+      <c r="N10" t="n">
         <v>12.050480343185328</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" t="n">
         <v>2024.0</v>
@@ -632,15 +665,18 @@
         <v>17.612016289105025</v>
       </c>
       <c r="L11" t="n">
+        <v>23.44217035343518</v>
+      </c>
+      <c r="M11" t="n">
         <v>-2.859895818483722</v>
       </c>
-      <c r="M11" t="n">
+      <c r="N11" t="n">
         <v>12.18814183977533</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" t="n">
         <v>2025.0</v>
@@ -673,15 +709,18 @@
         <v>15.578475099675297</v>
       </c>
       <c r="L12" t="n">
+        <v>23.3671070308337</v>
+      </c>
+      <c r="M12" t="n">
         <v>-3.0960360350975877</v>
       </c>
-      <c r="M12" t="n">
+      <c r="N12" t="n">
         <v>12.291253402990279</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" t="n">
         <v>2026.0</v>
@@ -714,15 +753,18 @@
         <v>13.510164139143443</v>
       </c>
       <c r="L13" t="n">
+        <v>23.312198344243047</v>
+      </c>
+      <c r="M13" t="n">
         <v>-3.335420296715994</v>
       </c>
-      <c r="M13" t="n">
+      <c r="N13" t="n">
         <v>12.370255967197156</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" t="n">
         <v>2027.0</v>
@@ -755,15 +797,18 @@
         <v>13.42093431498204</v>
       </c>
       <c r="L14" t="n">
+        <v>23.263882615521844</v>
+      </c>
+      <c r="M14" t="n">
         <v>-3.4133284139292313</v>
       </c>
-      <c r="M14" t="n">
+      <c r="N14" t="n">
         <v>12.41647092151446</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" t="n">
         <v>2028.0</v>
@@ -796,15 +841,18 @@
         <v>14.560764070970103</v>
       </c>
       <c r="L15" t="n">
+        <v>23.218591402403977</v>
+      </c>
+      <c r="M15" t="n">
         <v>-3.38843123256155</v>
       </c>
-      <c r="M15" t="n">
+      <c r="N15" t="n">
         <v>12.453170272975848</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" t="n">
         <v>2029.0</v>
@@ -837,15 +885,18 @@
         <v>14.473837088118286</v>
       </c>
       <c r="L16" t="n">
+        <v>23.172250822721104</v>
+      </c>
+      <c r="M16" t="n">
         <v>-3.456778218416834</v>
       </c>
-      <c r="M16" t="n">
+      <c r="N16" t="n">
         <v>12.494555073939033</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" t="n">
         <v>2030.0</v>
@@ -878,15 +929,18 @@
         <v>14.416844334742187</v>
       </c>
       <c r="L17" t="n">
+        <v>23.12171489691118</v>
+      </c>
+      <c r="M17" t="n">
         <v>-3.5256227347904674</v>
       </c>
-      <c r="M17" t="n">
+      <c r="N17" t="n">
         <v>12.531281168603005</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18" t="n">
         <v>2031.0</v>
@@ -919,15 +973,18 @@
         <v>14.557133064761809</v>
       </c>
       <c r="L18" t="n">
+        <v>23.083072685749684</v>
+      </c>
+      <c r="M18" t="n">
         <v>-3.570561558644269</v>
       </c>
-      <c r="M18" t="n">
+      <c r="N18" t="n">
         <v>12.560029926103743</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19" t="n">
         <v>2032.0</v>
@@ -960,15 +1017,18 @@
         <v>12.833952317015992</v>
       </c>
       <c r="L19" t="n">
+        <v>23.063830279312587</v>
+      </c>
+      <c r="M19" t="n">
         <v>-3.7510481546668597</v>
       </c>
-      <c r="M19" t="n">
+      <c r="N19" t="n">
         <v>12.582412586978915</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B20" t="n">
         <v>2033.0</v>
@@ -1001,15 +1061,18 @@
         <v>11.810585225999393</v>
       </c>
       <c r="L20" t="n">
+        <v>23.066955719892295</v>
+      </c>
+      <c r="M20" t="n">
         <v>-3.87211866543616</v>
       </c>
-      <c r="M20" t="n">
+      <c r="N20" t="n">
         <v>12.584424255143524</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21" t="n">
         <v>2034.0</v>
@@ -1042,15 +1105,18 @@
         <v>15.419172031115922</v>
       </c>
       <c r="L21" t="n">
+        <v>23.094765407588657</v>
+      </c>
+      <c r="M21" t="n">
         <v>-3.6217132809770023</v>
       </c>
-      <c r="M21" t="n">
+      <c r="N21" t="n">
         <v>12.576985122169999</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B22" t="n">
         <v>2035.0</v>
@@ -1083,15 +1149,18 @@
         <v>16.66987085518552</v>
       </c>
       <c r="L22" t="n">
+        <v>23.148986663035576</v>
+      </c>
+      <c r="M22" t="n">
         <v>-3.54597586612656</v>
       </c>
-      <c r="M22" t="n">
+      <c r="N22" t="n">
         <v>12.612057793068196</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B23" t="n">
         <v>2036.0</v>
@@ -1124,15 +1193,18 @@
         <v>15.449047401615925</v>
       </c>
       <c r="L23" t="n">
+        <v>23.190462502906957</v>
+      </c>
+      <c r="M23" t="n">
         <v>-3.6533307865743097</v>
       </c>
-      <c r="M23" t="n">
+      <c r="N23" t="n">
         <v>12.645977245564282</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24" t="n">
         <v>2037.0</v>
@@ -1165,15 +1237,18 @@
         <v>17.268501482228647</v>
       </c>
       <c r="L24" t="n">
+        <v>23.21770097078383</v>
+      </c>
+      <c r="M24" t="n">
         <v>-3.515789913860119</v>
       </c>
-      <c r="M24" t="n">
+      <c r="N24" t="n">
         <v>12.65453494549123</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25" t="n">
         <v>2038.0</v>
@@ -1206,15 +1281,18 @@
         <v>16.057711746298143</v>
       </c>
       <c r="L25" t="n">
+        <v>23.23199203759563</v>
+      </c>
+      <c r="M25" t="n">
         <v>-3.6063347356694004</v>
       </c>
-      <c r="M25" t="n">
+      <c r="N25" t="n">
         <v>12.671473220380463</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B26" t="n">
         <v>2039.0</v>
@@ -1247,15 +1325,18 @@
         <v>16.426786817660233</v>
       </c>
       <c r="L26" t="n">
+        <v>23.232307808184533</v>
+      </c>
+      <c r="M26" t="n">
         <v>-3.571765245142313</v>
       </c>
-      <c r="M26" t="n">
+      <c r="N26" t="n">
         <v>12.667774855802431</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B27" t="n">
         <v>2040.0</v>
@@ -1288,15 +1369,18 @@
         <v>15.30139786847719</v>
       </c>
       <c r="L27" t="n">
+        <v>23.226882343745693</v>
+      </c>
+      <c r="M27" t="n">
         <v>-3.6557998770034508</v>
       </c>
-      <c r="M27" t="n">
+      <c r="N27" t="n">
         <v>12.663209403589534</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B28" t="n">
         <v>2041.0</v>
@@ -1329,15 +1413,18 @@
         <v>13.776889568940124</v>
       </c>
       <c r="L28" t="n">
+        <v>23.222376915918186</v>
+      </c>
+      <c r="M28" t="n">
         <v>-3.7662517583821176</v>
       </c>
-      <c r="M28" t="n">
+      <c r="N28" t="n">
         <v>12.643083004647547</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B29" t="n">
         <v>2042.0</v>
@@ -1370,15 +1457,18 @@
         <v>13.78125167207902</v>
       </c>
       <c r="L29" t="n">
+        <v>23.219641831854</v>
+      </c>
+      <c r="M29" t="n">
         <v>-3.754457948608667</v>
       </c>
-      <c r="M29" t="n">
+      <c r="N29" t="n">
         <v>12.606502891806635</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B30" t="n">
         <v>2043.0</v>
@@ -1411,15 +1501,18 @@
         <v>13.775706050539645</v>
       </c>
       <c r="L30" t="n">
+        <v>23.217573735946473</v>
+      </c>
+      <c r="M30" t="n">
         <v>-3.738458312570659</v>
       </c>
-      <c r="M30" t="n">
+      <c r="N30" t="n">
         <v>12.570241262045338</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B31" t="n">
         <v>2044.0</v>
@@ -1452,9 +1545,12 @@
         <v>13.766490746207635</v>
       </c>
       <c r="L31" t="n">
+        <v>23.21963912026572</v>
+      </c>
+      <c r="M31" t="n">
         <v>-3.7190000477571576</v>
       </c>
-      <c r="M31" t="n">
+      <c r="N31" t="n">
         <v>12.537359395437909</v>
       </c>
     </row>
@@ -1509,10 +1605,13 @@
       <c r="M1" t="s">
         <v>11</v>
       </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" t="n">
         <v>2015.0</v>
@@ -1545,15 +1644,18 @@
         <v>31.43888383974378</v>
       </c>
       <c r="L2" t="n">
+        <v>28.233351474359893</v>
+      </c>
+      <c r="M2" t="n">
         <v>-1.6694337658040215</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>12.26596018288873</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="n">
         <v>2020.0</v>
@@ -1586,15 +1688,18 @@
         <v>21.15083417394243</v>
       </c>
       <c r="L3" t="n">
+        <v>23.785146651455086</v>
+      </c>
+      <c r="M3" t="n">
         <v>-2.2477383265021826</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>11.567780073910502</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="n">
         <v>2025.0</v>
@@ -1627,15 +1732,18 @@
         <v>15.578475099675297</v>
       </c>
       <c r="L4" t="n">
+        <v>23.3671070308337</v>
+      </c>
+      <c r="M4" t="n">
         <v>-3.0960360350975877</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>12.291253402990279</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" t="n">
         <v>2030.0</v>
@@ -1668,15 +1776,18 @@
         <v>14.416844334742187</v>
       </c>
       <c r="L5" t="n">
+        <v>23.12171489691118</v>
+      </c>
+      <c r="M5" t="n">
         <v>-3.5256227347904674</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>12.531281168603005</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="n">
         <v>2035.0</v>
@@ -1709,15 +1820,18 @@
         <v>16.66987085518552</v>
       </c>
       <c r="L6" t="n">
+        <v>23.148986663035576</v>
+      </c>
+      <c r="M6" t="n">
         <v>-3.54597586612656</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
         <v>12.612057793068196</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" t="n">
         <v>2040.0</v>
@@ -1750,15 +1864,18 @@
         <v>15.30139786847719</v>
       </c>
       <c r="L7" t="n">
+        <v>23.226882343745693</v>
+      </c>
+      <c r="M7" t="n">
         <v>-3.6557998770034508</v>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
         <v>12.663209403589534</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" t="n">
         <v>2044.0</v>
@@ -1791,9 +1908,12 @@
         <v>13.766490746207635</v>
       </c>
       <c r="L8" t="n">
+        <v>23.21963912026572</v>
+      </c>
+      <c r="M8" t="n">
         <v>-3.7190000477571576</v>
       </c>
-      <c r="M8" t="n">
+      <c r="N8" t="n">
         <v>12.537359395437909</v>
       </c>
     </row>

</xml_diff>